<commit_message>
AG: se borran las muestras ENDI mientras se define como se realizará el operativo
</commit_message>
<xml_diff>
--- a/productos/01_general/bitcora_marco.xlsx
+++ b/productos/01_general/bitcora_marco.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>version</t>
   </si>
@@ -56,6 +56,51 @@
   </si>
   <si>
     <t>OMAR LLAMBO</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Selección ENDI año 3</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>Selección ENCIET 202410</t>
+  </si>
+  <si>
+    <t>Rafael Encalada</t>
+  </si>
+  <si>
+    <t>Selección ENCIET 202411</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Selección ENCIET 202412</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Selección ENDI año 3 6 viv</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Selección ENDI año 3 7 viv</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Borrado selección ENDI 3 muestras</t>
   </si>
 </sst>
 </file>
@@ -120,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -138,6 +183,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,24 +489,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="E12:F12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -482,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -505,12 +552,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3">
-        <v>46199</v>
+        <v>45469</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>12</v>
@@ -526,6 +573,86 @@
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8">
+        <v>45671</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
seleccion enciet febrero 2025
</commit_message>
<xml_diff>
--- a/productos/01_general/bitcora_marco.xlsx
+++ b/productos/01_general/bitcora_marco.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>version</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>Borrado selección ENDI 3 muestras</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Selección ENCIET 202502</t>
   </si>
 </sst>
 </file>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +661,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="8">
+        <v>45674</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>